<commit_message>
Fixed failing valuation test - finally.  thinking about refactoring around factories
</commit_message>
<xml_diff>
--- a/BusinessLogicTests/Docs/ValuationChecker.xlsx
+++ b/BusinessLogicTests/Docs/ValuationChecker.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LEARNINGANDRAND\PortfolioManager\BusinessLogicTests\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,8 +33,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,7 +125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -165,7 +160,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,64 +337,64 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:8">
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8">
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8">
       <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8">
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8">
       <c r="F6">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8">
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8">
         <f>SUM(D2:D7)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <f>SUM(E2:E7)</f>
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="F8">
         <f>SUM(F2:F7)</f>
@@ -411,21 +406,21 @@
       </c>
       <c r="H8">
         <f>D8+E8+F8+G8</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8">
       <c r="D10">
         <f>D8/$H$8</f>
-        <v>7.1428571428571425E-2</v>
+        <v>0.2</v>
       </c>
       <c r="E10">
         <f>E8/$H$8</f>
-        <v>0.21428571428571427</v>
+        <v>0.6</v>
       </c>
       <c r="F10">
         <f>F8/$H$8</f>
-        <v>0.7142857142857143</v>
+        <v>0.2</v>
       </c>
       <c r="G10">
         <f>G8/$H$8</f>

</xml_diff>